<commit_message>
Implemented data driven approach
</commit_message>
<xml_diff>
--- a/src/main/java/com/mvmt/testdata/MVMT_DATA.xlsx
+++ b/src/main/java/com/mvmt/testdata/MVMT_DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/topb/Desktop/Automation Testing/Web Testing/MVMT_Automation/src/main/java/com/mvmt/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47124322-ABA7-DB42-B539-EDA9BD4B6E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B044B3FA-F628-684C-B52F-47035038D663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3872B4FA-B53F-DF4E-BF65-BAD340EFCF7B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -43,16 +43,22 @@
     <t>Password</t>
   </si>
   <si>
-    <t>justhustling39@gmail.com</t>
-  </si>
-  <si>
-    <t>Handmade8SermonHunter</t>
-  </si>
-  <si>
-    <t>hedinaookit@gmail.com</t>
-  </si>
-  <si>
-    <t>Udsdssble9Hapsee</t>
+    <t>user1@gmail.com</t>
+  </si>
+  <si>
+    <t>ThisIsUser1Pass</t>
+  </si>
+  <si>
+    <t>user2@gmail.com</t>
+  </si>
+  <si>
+    <t>ThisIsUser2Pass</t>
+  </si>
+  <si>
+    <t>ThisIsUser3Pass</t>
+  </si>
+  <si>
+    <t>user3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -97,10 +103,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3A6BFC-1E55-224C-A07B-CE8EB4250EF4}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,15 +453,25 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{AC4F5567-D08E-6548-A362-FC1509278B27}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{F644DD11-F2E1-B144-B27E-A1676CF3653B}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{F644DD11-F2E1-B144-B27E-A1676CF3653B}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{1C498547-DC9E-0A4B-8482-17748BEF6E87}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{B493774B-D1E8-AF4E-BF7F-66B9922344FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>